<commit_message>
all functionalities for cs50 project implemented
</commit_message>
<xml_diff>
--- a/finances_BF.xlsx
+++ b/finances_BF.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,12 +467,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>-$20.3</t>
+          <t>-$3</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>someone</t>
+          <t>store 1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -480,7 +480,281 @@
           <t>Ximena Leyva</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>9/17/2022</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>-$53.89</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Target</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Ximena Leyva</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Drinks for party</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>9/27/2022</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>-$43.78</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>another store</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Ximena Leyva</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>10/8/2022</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>-$73</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>a place</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Ximena Leyva</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>10/27/2022</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>-$142</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>shoe store</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Ximena Leyva</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>shoes</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>11/8/2022</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>-$34</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>make up store</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Ximena Leyva</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>10/5/2022</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>+$430</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>funding 2</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Ximena Leyva</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>11/10/2022</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>+$534</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>source 4</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Ximena Leyva</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>9/9/2022</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>+$24</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>donation</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Ximena Leyva</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>11/1/2022</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>+$1000</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>CPA</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Ximena Leyva</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>12/18/2022</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>+$2500</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>massive donation</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Ximena Leyva</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
final touches and md files
</commit_message>
<xml_diff>
--- a/finances_BF.xlsx
+++ b/finances_BF.xlsx
@@ -467,7 +467,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>-$3</t>
+          <t>-3</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -489,17 +489,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>9/17/2022</t>
+          <t>9/27/2022</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>-$53.89</t>
+          <t>-43.78</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Target</t>
+          <t>another store</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -509,24 +509,24 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Drinks for party</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>9/27/2022</t>
+          <t>10/27/2022</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>-$43.78</t>
+          <t>-142</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>another store</t>
+          <t>shoe store</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -536,24 +536,24 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>shoes</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>10/8/2022</t>
+          <t>11/8/2022</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>-$73</t>
+          <t>-34</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>a place</t>
+          <t>make up store</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -570,17 +570,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>10/27/2022</t>
+          <t>12/3/2022</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>-$142</t>
+          <t>-45</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>shoe store</t>
+          <t>store1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -590,24 +590,24 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>shoes</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>11/8/2022</t>
+          <t>10/5/2022</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>-$34</t>
+          <t>+430</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>make up store</t>
+          <t>funding 2</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -624,17 +624,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>10/5/2022</t>
+          <t>11/10/2022</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>+$430</t>
+          <t>+534</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>funding 2</t>
+          <t>source 4</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -651,17 +651,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>11/10/2022</t>
+          <t>9/9/2022</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>+$534</t>
+          <t>+24</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>source 4</t>
+          <t>donation</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -678,17 +678,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>9/9/2022</t>
+          <t>11/1/2022</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>+$24</t>
+          <t>+1000</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>donation</t>
+          <t>CPA</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -705,17 +705,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>11/1/2022</t>
+          <t>12/18/2022</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>+$1000</t>
+          <t>+2500</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CPA</t>
+          <t>massive donation</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -732,17 +732,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>12/18/2022</t>
+          <t>12/11/2022</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>+$2500</t>
+          <t>+430</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>massive donation</t>
+          <t>cpa</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">

</xml_diff>